<commit_message>
Fixes for timeshift run, PAS-15907: added to buglist
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/Refreshable_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/Refreshable_CA_CHOICE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSAA\CODE\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed cachemanager and refreshable
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/Refreshable_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/Refreshable_CA_CHOICE.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="61">
   <si>
     <t>VIN</t>
   </si>
@@ -122,18 +122,12 @@
     <t>TOYT</t>
   </si>
   <si>
-    <t>CAMRY</t>
-  </si>
-  <si>
     <t>CAMRY LE/XLE/SE</t>
   </si>
   <si>
     <t>4D SED</t>
   </si>
   <si>
-    <t>SEDAN 4 DOOR</t>
-  </si>
-  <si>
     <t>SED</t>
   </si>
   <si>
@@ -210,6 +204,9 @@
   </si>
   <si>
     <t>CA_MAKE_TEXT</t>
+  </si>
+  <si>
+    <t>COUPE</t>
   </si>
 </sst>
 </file>
@@ -551,7 +548,7 @@
   <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF7" sqref="AF7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,7 +595,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -670,28 +667,28 @@
         <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
@@ -699,7 +696,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="3">
         <v>2018</v>
@@ -708,30 +705,30 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="H2" s="3">
         <v>20000</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O2" s="3">
         <v>4</v>
@@ -739,28 +736,28 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S2" s="3">
         <v>2</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V2" s="3">
         <v>2</v>
       </c>
       <c r="W2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="Z2" s="3">
         <v>11</v>
@@ -787,7 +784,7 @@
         <v>20000101</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>28</v>
@@ -801,7 +798,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="3">
         <v>2018</v>
@@ -810,10 +807,10 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>27</v>
@@ -834,10 +831,10 @@
         <v>27</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O3" s="3">
         <v>4</v>
@@ -845,28 +842,28 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S3" s="3">
         <v>2</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V3" s="3">
         <v>2</v>
       </c>
       <c r="W3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="Z3" s="3">
         <v>12</v>
@@ -878,16 +875,16 @@
         <v>28</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AG3">
         <v>20010101</v>
@@ -907,7 +904,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3">
         <v>2018</v>
@@ -916,7 +913,7 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>27</v>
@@ -940,10 +937,10 @@
         <v>27</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O4" s="3">
         <v>4</v>
@@ -951,28 +948,28 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S4" s="3">
         <v>2</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V4" s="3">
         <v>2</v>
       </c>
       <c r="W4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="Z4" s="3">
         <v>12</v>
@@ -984,22 +981,22 @@
         <v>28</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AG4">
         <v>20130101</v>
       </c>
       <c r="AH4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AI4" t="s">
         <v>28</v>
@@ -1013,7 +1010,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3">
         <v>2018</v>
@@ -1022,10 +1019,10 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>27</v>
@@ -1046,10 +1043,10 @@
         <v>27</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O5" s="3">
         <v>4</v>
@@ -1057,28 +1054,28 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S5" s="3">
         <v>2</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V5" s="3">
         <v>2</v>
       </c>
       <c r="W5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="Z5" s="3">
         <v>12</v>
@@ -1090,22 +1087,22 @@
         <v>28</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AG5">
         <v>20150101</v>
       </c>
       <c r="AH5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AI5" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Fixed UpdatedVinRenewal Tests to use valid VIN data and reset to original values afterwards
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/Refreshable_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/Refreshable_CA_CHOICE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Reps\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -116,9 +116,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>4T1BE30K&amp;6</t>
-  </si>
-  <si>
     <t>TOYT</t>
   </si>
   <si>
@@ -200,13 +197,16 @@
     <t>MAKE_TEXT</t>
   </si>
   <si>
-    <t>TOYOTA</t>
-  </si>
-  <si>
     <t>CA_MAKE_TEXT</t>
   </si>
   <si>
     <t>COUPE</t>
+  </si>
+  <si>
+    <t>5TFUY5F1&amp;D</t>
+  </si>
+  <si>
+    <t>TOYOTA_UPDATED</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,7 +595,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -667,68 +667,68 @@
         <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3">
         <v>2018</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="H2" s="3">
         <v>20000</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="O2" s="3">
         <v>4</v>
@@ -736,28 +736,28 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S2" s="3">
         <v>2</v>
       </c>
       <c r="T2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="V2" s="3">
         <v>2</v>
       </c>
       <c r="W2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Z2" s="3">
         <v>11</v>
@@ -784,7 +784,7 @@
         <v>20000101</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>28</v>
@@ -795,10 +795,10 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3">
         <v>2018</v>
@@ -807,10 +807,10 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>27</v>
@@ -831,10 +831,10 @@
         <v>27</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="O3" s="3">
         <v>4</v>
@@ -842,28 +842,28 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S3" s="3">
         <v>2</v>
       </c>
       <c r="T3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="V3" s="3">
         <v>2</v>
       </c>
       <c r="W3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Z3" s="3">
         <v>12</v>
@@ -875,16 +875,16 @@
         <v>28</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG3">
         <v>20010101</v>
@@ -901,10 +901,10 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3">
         <v>2018</v>
@@ -913,7 +913,7 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>27</v>
@@ -937,10 +937,10 @@
         <v>27</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="O4" s="3">
         <v>4</v>
@@ -948,28 +948,28 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S4" s="3">
         <v>2</v>
       </c>
       <c r="T4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="V4" s="3">
         <v>2</v>
       </c>
       <c r="W4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Z4" s="3">
         <v>12</v>
@@ -981,22 +981,22 @@
         <v>28</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AG4">
         <v>20130101</v>
       </c>
       <c r="AH4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AI4" t="s">
         <v>28</v>
@@ -1007,10 +1007,10 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3">
         <v>2018</v>
@@ -1019,10 +1019,10 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>27</v>
@@ -1043,10 +1043,10 @@
         <v>27</v>
       </c>
       <c r="M5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="O5" s="3">
         <v>4</v>
@@ -1054,28 +1054,28 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S5" s="3">
         <v>2</v>
       </c>
       <c r="T5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="V5" s="3">
         <v>2</v>
       </c>
       <c r="W5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Z5" s="3">
         <v>12</v>
@@ -1087,22 +1087,22 @@
         <v>28</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG5">
         <v>20150101</v>
       </c>
       <c r="AH5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AI5" t="s">
         <v>28</v>

</xml_diff>